<commit_message>
set score excel upload visible
</commit_message>
<xml_diff>
--- a/TOYOTA.Web/src/TOYOTA.Web/wwwroot/Template/得分登记模板.xlsx
+++ b/TOYOTA.Web/src/TOYOTA.Web/wwwroot/Template/得分登记模板.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="14805" windowHeight="7980" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="14805" windowHeight="7980"/>
   </bookViews>
   <sheets>
     <sheet name="Score" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,169 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>作者</author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>得分
+0：不得分
+1：得分
+99：不涉及</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>通过与否
+0：不通过
+1：通过</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>在计划任务导入页面，点开计划任务详细页面中查找要登记得分的任务Id</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>在任务卡导入页面，找到对应的任务卡，点击详细页面，查找体系Id</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>数据来源类型
+D:巡视检核</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>作者</author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>检查结果，填入0或1
+0代表不合格
+1代表合格</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>同上一个sheet的计划任务下的任务卡Id</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>同上一次sheet 的体系Id</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>在任务卡导入页面，找到对应的任务卡，点击详细页面，查找对应的检查标准Id</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
@@ -133,7 +296,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,6 +319,14 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -481,11 +652,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -566,15 +737,16 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -611,5 +783,6 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>